<commit_message>
modif backend config database
</commit_message>
<xml_diff>
--- a/Documentation/Porduct-backlog-VITA-FORMA.xlsx
+++ b/Documentation/Porduct-backlog-VITA-FORMA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selsebil\Documents\Jemeremetsausport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selsebil\Documents\Jemeremetsausport\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519A61BF-9A2F-4304-AAF0-59ABF8A0CC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06EAED1-0A25-4E65-ADD6-F845C4985961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF1472C-DD9A-4D79-96F8-881C45860572}"/>
   </bookViews>
@@ -306,6 +306,36 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -314,36 +344,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF7112B-CEA8-472E-A8C8-93D553FB974F}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,370 +694,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="82" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8">
+      <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
+      <c r="A14" s="3">
         <v>10</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="10">
+      <c r="A15" s="7">
         <v>11</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
+      <c r="A16" s="5">
         <v>12</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
+      <c r="A17" s="3">
         <v>13</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+      <c r="A18" s="3">
         <v>14</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+      <c r="A19" s="3">
         <v>15</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
+      <c r="A20" s="3">
         <v>16</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+      <c r="A21" s="3">
         <v>17</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
+      <c r="A22" s="3">
         <v>18</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="13"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
-        <v>19</v>
-      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>